<commit_message>
Implement piecewise linear cost function
</commit_message>
<xml_diff>
--- a/superstructureIO.xlsx
+++ b/superstructureIO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1370831\Dropbox\PhD\Python\Pyomo\MyMILPFramework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1370831\Documents\GitHub\gotMilp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180" tabRatio="781"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180" tabRatio="840"/>
   </bookViews>
   <sheets>
     <sheet name="Conversion" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="CoolMatrix" sheetId="7" r:id="rId6"/>
     <sheet name="ElectricityMatrix" sheetId="8" r:id="rId7"/>
     <sheet name="Economic" sheetId="5" r:id="rId8"/>
+    <sheet name="TestConversionIO" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="60">
   <si>
     <t>t</t>
   </si>
@@ -126,9 +127,6 @@
     <t>u2</t>
   </si>
   <si>
-    <t>I0</t>
-  </si>
-  <si>
     <t>I1</t>
   </si>
   <si>
@@ -166,6 +164,54 @@
   </si>
   <si>
     <t>th-efficiency</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>IO</t>
+  </si>
+  <si>
+    <t>BOI</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Heat</t>
+  </si>
+  <si>
+    <t>CHP</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Cool</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>STS</t>
+  </si>
+  <si>
+    <t>LTS</t>
+  </si>
+  <si>
+    <t>IX1</t>
+  </si>
+  <si>
+    <t>IX2</t>
   </si>
 </sst>
 </file>
@@ -483,21 +529,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="12" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -511,10 +558,10 @@
         <v>16</v>
       </c>
       <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
         <v>43</v>
-      </c>
-      <c r="F1" t="s">
-        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>17</v>
@@ -538,37 +585,40 @@
         <v>27</v>
       </c>
       <c r="N1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
         <v>31</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>34</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" t="s">
         <v>35</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>36</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>37</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>38</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>39</v>
       </c>
-      <c r="W1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -624,15 +674,30 @@
       <c r="R2">
         <v>379580</v>
       </c>
+      <c r="S2">
+        <f>N2</f>
+        <v>31859</v>
+      </c>
+      <c r="T2">
+        <f>Q2</f>
+        <v>14000</v>
+      </c>
       <c r="U2">
+        <f>R2</f>
+        <v>379580</v>
+      </c>
+      <c r="V2">
         <f>(R2-P2)/(Q2-O2)</f>
         <v>24.837194244604316</v>
       </c>
       <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -688,15 +753,30 @@
       <c r="R3">
         <v>379580</v>
       </c>
+      <c r="S3">
+        <f>N3</f>
+        <v>31859</v>
+      </c>
+      <c r="T3">
+        <f>Q3</f>
+        <v>14000</v>
+      </c>
       <c r="U3">
-        <f t="shared" ref="U3:U9" si="1">(R3-P3)/(Q3-O3)</f>
+        <f>R3</f>
+        <v>379580</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V9" si="1">(R3-P3)/(Q3-O3)</f>
         <v>24.837194244604316</v>
       </c>
       <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -752,15 +832,28 @@
       <c r="R4">
         <v>278644</v>
       </c>
+      <c r="S4">
+        <v>114976</v>
+      </c>
+      <c r="T4">
+        <v>3200</v>
+      </c>
       <c r="U4">
-        <f t="shared" si="1"/>
+        <v>850563</v>
+      </c>
+      <c r="V4">
+        <f>(R4-P4)/(Q4-O4)</f>
         <v>229.34905660377359</v>
       </c>
       <c r="W4">
+        <f>(U4-R4)/(T4-Q4)</f>
+        <v>229.87098070739549</v>
+      </c>
+      <c r="X4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -816,15 +909,28 @@
       <c r="R5">
         <v>278644</v>
       </c>
+      <c r="S5">
+        <v>114976</v>
+      </c>
+      <c r="T5">
+        <v>3200</v>
+      </c>
       <c r="U5">
+        <v>850563</v>
+      </c>
+      <c r="V5">
         <f t="shared" si="1"/>
         <v>229.34905660377359</v>
       </c>
       <c r="W5">
+        <f t="shared" ref="W3:W9" si="2">(U5-R5)/(T5-Q5)</f>
+        <v>229.87098070739549</v>
+      </c>
+      <c r="X5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -880,15 +986,28 @@
       <c r="R6">
         <v>154012</v>
       </c>
+      <c r="S6">
+        <v>105929</v>
+      </c>
+      <c r="T6">
+        <v>6500</v>
+      </c>
       <c r="U6">
+        <v>522651</v>
+      </c>
+      <c r="V6">
         <f t="shared" si="1"/>
         <v>122.17</v>
       </c>
       <c r="W6">
+        <f t="shared" si="2"/>
+        <v>64.111130434782609</v>
+      </c>
+      <c r="X6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -944,15 +1063,28 @@
       <c r="R7">
         <v>154012</v>
       </c>
+      <c r="S7">
+        <v>105929</v>
+      </c>
+      <c r="T7">
+        <v>6500</v>
+      </c>
       <c r="U7">
+        <v>522651</v>
+      </c>
+      <c r="V7">
         <f t="shared" si="1"/>
         <v>122.17</v>
       </c>
       <c r="W7">
+        <f t="shared" si="2"/>
+        <v>64.111130434782609</v>
+      </c>
+      <c r="X7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1008,15 +1140,30 @@
       <c r="R8">
         <v>1572302</v>
       </c>
+      <c r="S8">
+        <f>N8</f>
+        <v>27202</v>
+      </c>
+      <c r="T8">
+        <f>Q8</f>
+        <v>10000</v>
+      </c>
       <c r="U8">
+        <f>R8</f>
+        <v>1572302</v>
+      </c>
+      <c r="V8">
         <f t="shared" si="1"/>
         <v>154.51</v>
       </c>
       <c r="W8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1072,11 +1219,26 @@
       <c r="R9">
         <v>1572302</v>
       </c>
+      <c r="S9">
+        <f>N9</f>
+        <v>27202</v>
+      </c>
+      <c r="T9">
+        <f>Q9</f>
+        <v>10000</v>
+      </c>
       <c r="U9">
+        <f>R9</f>
+        <v>1572302</v>
+      </c>
+      <c r="V9">
         <f t="shared" si="1"/>
         <v>154.51</v>
       </c>
       <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
         <v>1</v>
       </c>
     </row>
@@ -1118,10 +1280,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
         <v>41</v>
-      </c>
-      <c r="E1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3412,4 +3574,176 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement piecewise performance function with ksi 1 and ksi 2
</commit_message>
<xml_diff>
--- a/superstructureIO.xlsx
+++ b/superstructureIO.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="64">
   <si>
     <t>t</t>
   </si>
@@ -109,15 +109,9 @@
     <t>CD</t>
   </si>
   <si>
-    <t>u0</t>
-  </si>
-  <si>
     <t>u1</t>
   </si>
   <si>
-    <t>performance-slope</t>
-  </si>
-  <si>
     <t>v1</t>
   </si>
   <si>
@@ -212,6 +206,24 @@
   </si>
   <si>
     <t>IX2</t>
+  </si>
+  <si>
+    <t>ux1</t>
+  </si>
+  <si>
+    <t>ux2</t>
+  </si>
+  <si>
+    <t>v3</t>
+  </si>
+  <si>
+    <t>u3</t>
+  </si>
+  <si>
+    <t>performance-slope-1</t>
+  </si>
+  <si>
+    <t>performance-slope-2</t>
   </si>
 </sst>
 </file>
@@ -529,22 +541,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="12" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="22" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -558,67 +569,79 @@
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
         <v>17</v>
       </c>
       <c r="H1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>63</v>
+      </c>
+      <c r="R1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="U1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="W1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Y1" t="s">
         <v>34</v>
       </c>
-      <c r="S1" t="s">
-        <v>59</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="Z1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AA1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AB1" t="s">
         <v>37</v>
       </c>
-      <c r="W1" t="s">
-        <v>38</v>
-      </c>
-      <c r="X1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -656,48 +679,63 @@
         <v>1.0004</v>
       </c>
       <c r="M2">
+        <f>H2</f>
+        <v>2.29E-2</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1.0004</v>
+      </c>
+      <c r="P2">
         <f>(L2-J2)/(K2-I2)</f>
         <v>0.97749999999999981</v>
       </c>
-      <c r="N2">
+      <c r="Q2">
+        <f>P2</f>
+        <v>0.97749999999999981</v>
+      </c>
+      <c r="R2">
         <v>31859</v>
       </c>
-      <c r="O2">
+      <c r="S2">
         <v>100</v>
       </c>
-      <c r="P2">
+      <c r="T2">
         <v>34343</v>
       </c>
-      <c r="Q2">
+      <c r="U2">
         <v>14000</v>
       </c>
-      <c r="R2">
+      <c r="V2">
         <v>379580</v>
       </c>
-      <c r="S2">
-        <f>N2</f>
+      <c r="W2">
+        <f>R2</f>
         <v>31859</v>
       </c>
-      <c r="T2">
-        <f>Q2</f>
+      <c r="X2">
+        <f>U2</f>
         <v>14000</v>
       </c>
-      <c r="U2">
-        <f>R2</f>
+      <c r="Y2">
+        <f>V2</f>
         <v>379580</v>
       </c>
-      <c r="V2">
-        <f>(R2-P2)/(Q2-O2)</f>
+      <c r="Z2">
+        <f>(V2-T2)/(U2-S2)</f>
         <v>24.837194244604316</v>
       </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
+      <c r="AA2">
+        <f>Z2</f>
+        <v>24.837194244604316</v>
+      </c>
+      <c r="AB2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -735,48 +773,63 @@
         <v>1.0004</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M9" si="0">(L3-J3)/(K3-I3)</f>
+        <f t="shared" ref="M3:M5" si="0">H3</f>
+        <v>2.29E-2</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1.0004</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P9" si="1">(L3-J3)/(K3-I3)</f>
         <v>0.97749999999999981</v>
       </c>
-      <c r="N3">
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q5" si="2">P3</f>
+        <v>0.97749999999999981</v>
+      </c>
+      <c r="R3">
         <v>31859</v>
       </c>
-      <c r="O3">
+      <c r="S3">
         <v>100</v>
       </c>
-      <c r="P3">
+      <c r="T3">
         <v>34343</v>
       </c>
-      <c r="Q3">
+      <c r="U3">
         <v>14000</v>
       </c>
-      <c r="R3">
+      <c r="V3">
         <v>379580</v>
       </c>
-      <c r="S3">
-        <f>N3</f>
+      <c r="W3">
+        <f>R3</f>
         <v>31859</v>
       </c>
-      <c r="T3">
-        <f>Q3</f>
+      <c r="X3">
+        <f>U3</f>
         <v>14000</v>
       </c>
-      <c r="U3">
-        <f>R3</f>
+      <c r="Y3">
+        <f>V3</f>
         <v>379580</v>
       </c>
-      <c r="V3">
-        <f t="shared" ref="V3:V9" si="1">(R3-P3)/(Q3-O3)</f>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z9" si="3">(V3-T3)/(U3-S3)</f>
         <v>24.837194244604316</v>
       </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3">
+      <c r="AA3">
+        <f>Z3</f>
+        <v>24.837194244604316</v>
+      </c>
+      <c r="AB3">
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -815,45 +868,59 @@
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
+        <v>-2.35E-2</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0.98150000000000004</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
         <v>1.0050000000000001</v>
       </c>
-      <c r="N4">
+      <c r="Q4">
+        <f t="shared" si="2"/>
+        <v>1.0050000000000001</v>
+      </c>
+      <c r="R4">
         <v>115347</v>
       </c>
-      <c r="O4">
+      <c r="S4">
         <v>500</v>
       </c>
-      <c r="P4">
+      <c r="T4">
         <v>230022</v>
       </c>
-      <c r="Q4">
+      <c r="U4">
         <v>712</v>
       </c>
-      <c r="R4">
+      <c r="V4">
         <v>278644</v>
       </c>
-      <c r="S4">
+      <c r="W4">
         <v>114976</v>
       </c>
-      <c r="T4">
+      <c r="X4">
         <v>3200</v>
       </c>
-      <c r="U4">
+      <c r="Y4">
         <v>850563</v>
       </c>
-      <c r="V4">
-        <f>(R4-P4)/(Q4-O4)</f>
+      <c r="Z4">
+        <f>(V4-T4)/(U4-S4)</f>
         <v>229.34905660377359</v>
       </c>
-      <c r="W4">
-        <f>(U4-R4)/(T4-Q4)</f>
+      <c r="AA4">
+        <f>(Y4-V4)/(X4-U4)</f>
         <v>229.87098070739549</v>
       </c>
-      <c r="X4">
+      <c r="AB4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -892,45 +959,59 @@
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
+        <v>-2.35E-2</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>0.98150000000000004</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
         <v>1.0050000000000001</v>
       </c>
-      <c r="N5">
+      <c r="Q5">
+        <f t="shared" si="2"/>
+        <v>1.0050000000000001</v>
+      </c>
+      <c r="R5">
         <v>115347</v>
       </c>
-      <c r="O5">
+      <c r="S5">
         <v>500</v>
       </c>
-      <c r="P5">
+      <c r="T5">
         <v>230022</v>
       </c>
-      <c r="Q5">
+      <c r="U5">
         <v>712</v>
       </c>
-      <c r="R5">
+      <c r="V5">
         <v>278644</v>
       </c>
-      <c r="S5">
+      <c r="W5">
         <v>114976</v>
       </c>
-      <c r="T5">
+      <c r="X5">
         <v>3200</v>
       </c>
-      <c r="U5">
+      <c r="Y5">
         <v>850563</v>
       </c>
-      <c r="V5">
-        <f t="shared" si="1"/>
+      <c r="Z5">
+        <f t="shared" si="3"/>
         <v>229.34905660377359</v>
       </c>
-      <c r="W5">
-        <f t="shared" ref="W3:W9" si="2">(U5-R5)/(T5-Q5)</f>
+      <c r="AA5">
+        <f t="shared" ref="AA5:AA7" si="4">(Y5-V5)/(X5-U5)</f>
         <v>229.87098070739549</v>
       </c>
-      <c r="X5">
+      <c r="AB5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -968,46 +1049,59 @@
         <v>0.48330000000000001</v>
       </c>
       <c r="M6">
-        <f t="shared" si="0"/>
+        <v>-0.26669999999999999</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0.98329999999999995</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="1"/>
         <v>0.52775000000000005</v>
       </c>
-      <c r="N6">
+      <c r="Q6">
+        <f t="shared" ref="Q6:Q9" si="5">(O6-L6)/(N6-K6)</f>
+        <v>1.2499999999999998</v>
+      </c>
+      <c r="R6">
         <v>62385</v>
       </c>
-      <c r="O6">
+      <c r="S6">
         <v>50</v>
       </c>
-      <c r="P6">
+      <c r="T6">
         <v>68493</v>
       </c>
-      <c r="Q6">
+      <c r="U6">
         <v>750</v>
       </c>
-      <c r="R6">
+      <c r="V6">
         <v>154012</v>
       </c>
-      <c r="S6">
+      <c r="W6">
         <v>105929</v>
       </c>
-      <c r="T6">
+      <c r="X6">
         <v>6500</v>
       </c>
-      <c r="U6">
+      <c r="Y6">
         <v>522651</v>
       </c>
-      <c r="V6">
-        <f t="shared" si="1"/>
+      <c r="Z6">
+        <f t="shared" si="3"/>
         <v>122.17</v>
       </c>
-      <c r="W6">
-        <f t="shared" si="2"/>
+      <c r="AA6">
+        <f t="shared" si="4"/>
         <v>64.111130434782609</v>
       </c>
-      <c r="X6">
+      <c r="AB6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1045,46 +1139,59 @@
         <v>0.48330000000000001</v>
       </c>
       <c r="M7">
-        <f t="shared" si="0"/>
+        <v>-0.26669999999999999</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0.98329999999999995</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
         <v>0.52775000000000005</v>
       </c>
-      <c r="N7">
+      <c r="Q7">
+        <f t="shared" si="5"/>
+        <v>1.2499999999999998</v>
+      </c>
+      <c r="R7">
         <v>62385</v>
       </c>
-      <c r="O7">
+      <c r="S7">
         <v>50</v>
       </c>
-      <c r="P7">
+      <c r="T7">
         <v>68493</v>
       </c>
-      <c r="Q7">
+      <c r="U7">
         <v>750</v>
       </c>
-      <c r="R7">
+      <c r="V7">
         <v>154012</v>
       </c>
-      <c r="S7">
+      <c r="W7">
         <v>105929</v>
       </c>
-      <c r="T7">
+      <c r="X7">
         <v>6500</v>
       </c>
-      <c r="U7">
+      <c r="Y7">
         <v>522651</v>
       </c>
-      <c r="V7">
-        <f t="shared" si="1"/>
+      <c r="Z7">
+        <f t="shared" si="3"/>
         <v>122.17</v>
       </c>
-      <c r="W7">
-        <f t="shared" si="2"/>
+      <c r="AA7">
+        <f t="shared" si="4"/>
         <v>64.111130434782609</v>
       </c>
-      <c r="X7">
+      <c r="AB7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1122,48 +1229,62 @@
         <v>0.59360000000000002</v>
       </c>
       <c r="M8">
-        <f t="shared" si="0"/>
+        <v>-0.3145</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0.98280000000000001</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
         <v>0.55020000000000013</v>
       </c>
-      <c r="N8">
+      <c r="Q8">
+        <f t="shared" si="5"/>
+        <v>1.297333333333333</v>
+      </c>
+      <c r="R8">
         <v>27202</v>
       </c>
-      <c r="O8">
+      <c r="S8">
         <v>400</v>
       </c>
-      <c r="P8">
+      <c r="T8">
         <v>89006</v>
       </c>
-      <c r="Q8">
+      <c r="U8">
         <v>10000</v>
       </c>
-      <c r="R8">
+      <c r="V8">
         <v>1572302</v>
       </c>
-      <c r="S8">
-        <f>N8</f>
+      <c r="W8">
+        <f>R8</f>
         <v>27202</v>
       </c>
-      <c r="T8">
-        <f>Q8</f>
+      <c r="X8">
+        <f>U8</f>
         <v>10000</v>
       </c>
-      <c r="U8">
-        <f>R8</f>
+      <c r="Y8">
+        <f>V8</f>
         <v>1572302</v>
       </c>
-      <c r="V8">
-        <f t="shared" si="1"/>
+      <c r="Z8">
+        <f t="shared" si="3"/>
         <v>154.51</v>
       </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="AA8">
+        <f>Z8</f>
+        <v>154.51</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1201,44 +1322,58 @@
         <v>0.59360000000000002</v>
       </c>
       <c r="M9">
-        <f t="shared" si="0"/>
+        <v>-0.3145</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0.98280000000000001</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
         <v>0.55020000000000013</v>
       </c>
-      <c r="N9">
+      <c r="Q9">
+        <f t="shared" si="5"/>
+        <v>1.297333333333333</v>
+      </c>
+      <c r="R9">
         <v>27202</v>
       </c>
-      <c r="O9">
+      <c r="S9">
         <v>400</v>
       </c>
-      <c r="P9">
+      <c r="T9">
         <v>89006</v>
       </c>
-      <c r="Q9">
+      <c r="U9">
         <v>10000</v>
       </c>
-      <c r="R9">
+      <c r="V9">
         <v>1572302</v>
       </c>
-      <c r="S9">
-        <f>N9</f>
+      <c r="W9">
+        <f>R9</f>
         <v>27202</v>
       </c>
-      <c r="T9">
-        <f>Q9</f>
+      <c r="X9">
+        <f>U9</f>
         <v>10000</v>
       </c>
-      <c r="U9">
-        <f>R9</f>
+      <c r="Y9">
+        <f>V9</f>
         <v>1572302</v>
       </c>
-      <c r="V9">
-        <f t="shared" si="1"/>
+      <c r="Z9">
+        <f t="shared" si="3"/>
         <v>154.51</v>
       </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
+      <c r="AA9">
+        <f>Z9</f>
+        <v>154.51</v>
+      </c>
+      <c r="AB9">
         <v>1</v>
       </c>
     </row>
@@ -1263,7 +1398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
@@ -1280,10 +1415,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3594,153 +3729,153 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SDO Operational optimisation only
</commit_message>
<xml_diff>
--- a/superstructureIO.xlsx
+++ b/superstructureIO.xlsx
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,7 +1481,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M13"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>